<commit_message>
Updated some ref des
</commit_message>
<xml_diff>
--- a/pcb/bom.xlsx
+++ b/pcb/bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\Projects\mppcHighVoltage\mppcHighVoltage\pcb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\OneDrive\projects\mppcHighVoltage\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="142">
   <si>
     <t>QTY</t>
   </si>
@@ -320,24 +320,12 @@
     <t>U2</t>
   </si>
   <si>
-    <t>C6</t>
-  </si>
-  <si>
     <t>C7</t>
   </si>
   <si>
     <t>C8</t>
   </si>
   <si>
-    <t>.1uF</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
     <t>RF Shield</t>
   </si>
   <si>
@@ -353,9 +341,6 @@
     <t>http://www.digikey.com/product-search/en/rf-if-and-rfid/rf-shields/3539677?k=&amp;pkeyword=&amp;pv577=1130&amp;pv1217=41&amp;FV=fff40036%2Cfff802dd%2Cfffc03b8&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
   </si>
   <si>
-    <t>10k 0.1%</t>
-  </si>
-  <si>
     <t>R2, R6</t>
   </si>
   <si>
@@ -368,9 +353,6 @@
     <t>10µF 6.3V Ceramic Capacitor X5R 0603</t>
   </si>
   <si>
-    <t>RX</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM155R71C104KA88J/490-6328-2-ND/2610892</t>
   </si>
   <si>
@@ -389,9 +371,6 @@
     <t>http://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM155R60G106ME44D/490-10693-2-ND/4905101</t>
   </si>
   <si>
-    <t>220k 1%</t>
-  </si>
-  <si>
     <t>RES SMD 220K OHM 1% 1/16W 0402</t>
   </si>
   <si>
@@ -401,9 +380,6 @@
     <t>RES SMD 270K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t>270k 1%</t>
-  </si>
-  <si>
     <t>RC0402FR-07270KL</t>
   </si>
   <si>
@@ -456,6 +432,27 @@
   </si>
   <si>
     <t>CPF0402B20RE1</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>HV Divider</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>C6, C10</t>
+  </si>
+  <si>
+    <t>Decoupling Capacitor</t>
   </si>
 </sst>
 </file>
@@ -624,6 +621,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -659,6 +673,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -814,7 +845,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,7 +898,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
         <v>39</v>
@@ -897,7 +928,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
         <v>52</v>
@@ -927,7 +958,7 @@
         <v>56</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D4" t="s">
         <v>55</v>
@@ -1161,10 +1192,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C12" t="s">
         <v>67</v>
@@ -1200,7 +1231,7 @@
         <v>83</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E13" t="s">
         <v>82</v>
@@ -1260,7 +1291,7 @@
         <v>80</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E15" t="s">
         <v>79</v>
@@ -1316,13 +1347,13 @@
       <c r="B17" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" t="s">
         <v>92</v>
       </c>
       <c r="F17" s="3">
@@ -1336,24 +1367,24 @@
         <v>1.3442000000000001</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>129</v>
+        <v>141</v>
+      </c>
+      <c r="C18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" t="s">
+        <v>121</v>
       </c>
       <c r="F18">
         <v>2</v>
@@ -1366,24 +1397,24 @@
         <v>9.5999999999999992E-3</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>139</v>
+        <v>109</v>
+      </c>
+      <c r="E19" t="s">
+        <v>131</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1396,24 +1427,24 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" t="s">
         <v>112</v>
       </c>
-      <c r="D20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>140</v>
+      <c r="E20" t="s">
+        <v>132</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1426,21 +1457,24 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>135</v>
+      </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E21" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1453,24 +1487,24 @@
         <v>3.53</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="B22" t="s">
-        <v>120</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>133</v>
+        <v>136</v>
+      </c>
+      <c r="C22" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" t="s">
+        <v>125</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1483,24 +1517,24 @@
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="B23" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" t="s">
         <v>124</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1513,24 +1547,24 @@
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>130</v>
+        <v>136</v>
+      </c>
+      <c r="C24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" t="s">
+        <v>122</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1543,7 +1577,7 @@
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Still 2016 version will likey change soon
</commit_message>
<xml_diff>
--- a/pcb/bom.xlsx
+++ b/pcb/bom.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\Projects\mppcHighVoltage\mppcHighVoltage\pcb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\OneDrive\projects\mppcHighVoltage\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="146">
   <si>
     <t>QTY</t>
   </si>
@@ -368,9 +368,6 @@
     <t>10µF 6.3V Ceramic Capacitor X5R 0603</t>
   </si>
   <si>
-    <t>RX</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM155R71C104KA88J/490-6328-2-ND/2610892</t>
   </si>
   <si>
@@ -456,6 +453,18 @@
   </si>
   <si>
     <t>CPF0402B20RE1</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R8</t>
   </si>
 </sst>
 </file>
@@ -621,6 +630,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -656,6 +682,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -811,7 +854,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,7 +907,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D2" t="s">
         <v>39</v>
@@ -894,7 +937,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D3" t="s">
         <v>52</v>
@@ -924,7 +967,7 @@
         <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D4" t="s">
         <v>55</v>
@@ -1197,7 +1240,7 @@
         <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E13" t="s">
         <v>82</v>
@@ -1257,7 +1300,7 @@
         <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E15" t="s">
         <v>79</v>
@@ -1347,10 +1390,10 @@
         <v>111</v>
       </c>
       <c r="D18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" t="s">
         <v>128</v>
-      </c>
-      <c r="E18" t="s">
-        <v>129</v>
       </c>
       <c r="F18">
         <v>2</v>
@@ -1363,7 +1406,7 @@
         <v>9.5999999999999992E-3</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1374,13 +1417,13 @@
         <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1393,7 +1436,7 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1407,10 +1450,10 @@
         <v>112</v>
       </c>
       <c r="D20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1423,10 +1466,13 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>142</v>
+      </c>
       <c r="B21" t="s">
         <v>103</v>
       </c>
@@ -1455,19 +1501,19 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="B22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" t="s">
         <v>120</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>121</v>
       </c>
-      <c r="D22" t="s">
-        <v>122</v>
-      </c>
       <c r="E22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1480,24 +1526,24 @@
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="B23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" t="s">
         <v>124</v>
       </c>
-      <c r="C23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" t="s">
-        <v>125</v>
-      </c>
       <c r="E23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1510,24 +1556,24 @@
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="B24" t="s">
         <v>108</v>
       </c>
       <c r="C24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" t="s">
         <v>126</v>
       </c>
-      <c r="D24" t="s">
-        <v>127</v>
-      </c>
       <c r="E24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1540,7 +1586,7 @@
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>